<commit_message>
aggiunti dati misuraione parabole
</commit_message>
<xml_diff>
--- a/KARTER/dati raccolti karter.xlsx
+++ b/KARTER/dati raccolti karter.xlsx
@@ -29,7 +29,7 @@
     <t>t3</t>
   </si>
   <si>
-    <t>m</t>
+    <t>d1(cm)</t>
   </si>
 </sst>
 </file>
@@ -67,9 +67,10 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,9 +876,9 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="14.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -887,9 +888,242 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.0211000000000001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.0550000000000002</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.0024000000000002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.9923999999999999</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.984</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.9245000000000001</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.9677</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.8697999999999999</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.9520999999999999</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.8317000000000001</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.9399</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.8089</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.9199999999999999</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.7956000000000001</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.9207000000000001</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.7916000000000001</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.9132</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.7964</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.9094</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.8058000000000001</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12">
+        <v>55</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.9077</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.8214999999999999</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13">
+        <v>60</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.9092</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.8411</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="2">
+        <v>65</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.9147000000000001</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.8643000000000001</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15">
+        <v>70</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.9245000000000001</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.8883000000000001</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="2">
+        <v>75</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.9368000000000001</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.9172</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17">
+        <v>80</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.9539</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.9458</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="2">
+        <v>85</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.9770000000000001</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.9756</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19">
+        <v>90</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2.0024000000000002</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2.0064000000000002</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
misura di g fatta
</commit_message>
<xml_diff>
--- a/KARTER/dati raccolti karter.xlsx
+++ b/KARTER/dati raccolti karter.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="misure grossolane" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="misure grossolane girate" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="misure_meno_grossolane" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="misure_intorno_sensibile" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="biglie caduta libera" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -57,21 +58,20 @@
     <t xml:space="preserve">AVG T</t>
   </si>
   <si>
-    <t xml:space="preserve">DEVSTD t</t>
+    <t>h</t>
   </si>
   <si>
-    <t xml:space="preserve">DEVSTD T</t>
+    <t>t5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="160" formatCode="0.0000"/>
-    <numFmt numFmtId="161" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -84,8 +84,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,6 +104,12 @@
         <bgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -108,22 +120,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="160" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1226,12 +1239,8 @@
       <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
+      <c r="L1"/>
+      <c r="M1"/>
     </row>
     <row r="2">
       <c r="A2" s="4">
@@ -1269,14 +1278,8 @@
         <f t="shared" ref="K2:K9" si="1">AVERAGE(F2:I2)</f>
         <v>2.01335</v>
       </c>
-      <c r="L2" s="6">
-        <f>STDEV(B2:E2)</f>
-        <v>0.00073484692283495303</v>
-      </c>
-      <c r="M2" s="6">
-        <f>STDEV(F2:I2)</f>
-        <v>0.00038729833462079462</v>
-      </c>
+      <c r="L2"/>
+      <c r="M2"/>
     </row>
     <row r="3">
       <c r="A3" s="4">
@@ -1314,14 +1317,8 @@
         <f t="shared" si="1"/>
         <v>2.012175</v>
       </c>
-      <c r="L3" s="6">
-        <f>STDEV(B3:E3)</f>
-        <v>0.00058022983951756368</v>
-      </c>
-      <c r="M3" s="6">
-        <f>STDEV(F3:I3)</f>
-        <v>0.00025000000000008349</v>
-      </c>
+      <c r="L3"/>
+      <c r="M3"/>
     </row>
     <row r="4">
       <c r="A4" s="4">
@@ -1359,14 +1356,8 @@
         <f t="shared" si="1"/>
         <v>2.0111999999999997</v>
       </c>
-      <c r="L4" s="6">
-        <f>STDEV(B4:E4)</f>
-        <v>0.0003162277660167563</v>
-      </c>
-      <c r="M4" s="6">
-        <f>STDEV(F4:I4)</f>
-        <v>0.00050332229568466117</v>
-      </c>
+      <c r="L4"/>
+      <c r="M4"/>
     </row>
     <row r="5">
       <c r="A5" s="4">
@@ -1404,14 +1395,8 @@
         <f t="shared" si="1"/>
         <v>2.0086750000000002</v>
       </c>
-      <c r="L5" s="6">
-        <f>STDEV(B5:E5)</f>
-        <v>0.00020000000000020002</v>
-      </c>
-      <c r="M5" s="6">
-        <f>STDEV(F5:I5)</f>
-        <v>0.00038622100754173911</v>
-      </c>
+      <c r="L5"/>
+      <c r="M5"/>
     </row>
     <row r="6">
       <c r="A6" s="4">
@@ -1449,14 +1434,8 @@
         <f t="shared" si="1"/>
         <v>2.0066250000000001</v>
       </c>
-      <c r="L6" s="6">
-        <f>STDEV(B6:E6)</f>
-        <v>0.00057445626465373967</v>
-      </c>
-      <c r="M6" s="6">
-        <f>STDEV(F6:I6)</f>
-        <v>4.9999999999883471e-05</v>
-      </c>
+      <c r="L6"/>
+      <c r="M6"/>
     </row>
     <row r="7">
       <c r="A7" s="4">
@@ -1494,14 +1473,8 @@
         <f t="shared" si="1"/>
         <v>2.003825</v>
       </c>
-      <c r="L7" s="6">
-        <f>STDEV(B7:E7)</f>
-        <v>0.00087368949480544128</v>
-      </c>
-      <c r="M7" s="6">
-        <f>STDEV(F7:I7)</f>
-        <v>0.00086938675704976293</v>
-      </c>
+      <c r="L7"/>
+      <c r="M7"/>
     </row>
     <row r="8">
       <c r="A8" s="4">
@@ -1539,14 +1512,8 @@
         <f t="shared" si="1"/>
         <v>2.002475</v>
       </c>
-      <c r="L8" s="6">
-        <f>STDEV(B8:E8)</f>
-        <v>0.0004349329450232945</v>
-      </c>
-      <c r="M8" s="6">
-        <f>STDEV(F8:I8)</f>
-        <v>0.00017078251276594198</v>
-      </c>
+      <c r="L8"/>
+      <c r="M8"/>
     </row>
     <row r="9">
       <c r="A9" s="4">
@@ -1584,14 +1551,8 @@
         <f t="shared" si="1"/>
         <v>2.0013000000000001</v>
       </c>
-      <c r="L9" s="6">
-        <f>STDEV(B9:E9)</f>
-        <v>0.00031091263510303336</v>
-      </c>
-      <c r="M9" s="6">
-        <f>STDEV(F9:I9)</f>
-        <v>0.00018257418583503526</v>
-      </c>
+      <c r="L9"/>
+      <c r="M9"/>
     </row>
     <row r="10">
       <c r="A10" s="4">
@@ -1629,44 +1590,48 @@
         <f>AVERAGE(F10:I10)</f>
         <v>1.9995250000000002</v>
       </c>
-      <c r="L10" s="6">
-        <f>STDEV(B10:E10)</f>
-        <v>0.0007937253933193877</v>
-      </c>
-      <c r="M10" s="6">
-        <f>STDEV(F10:I10)</f>
-        <v>0.00024999999999997247</v>
-      </c>
+      <c r="L10"/>
+      <c r="M10"/>
     </row>
     <row r="11">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
+      <c r="L11"/>
+      <c r="M11"/>
     </row>
     <row r="12">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
+      <c r="L12"/>
+      <c r="M12"/>
     </row>
     <row r="13">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
+      <c r="L13"/>
+      <c r="M13"/>
     </row>
     <row r="14">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
+      <c r="L14"/>
+      <c r="M14"/>
     </row>
     <row r="15">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
+      <c r="L15"/>
+      <c r="M15"/>
     </row>
     <row r="16">
       <c r="B16" s="1"/>
@@ -1698,6 +1663,74 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>